<commit_message>
[UPDATE] reactions validation + [FIX] simulation_sp
</commit_message>
<xml_diff>
--- a/Validation/produced_at_day.xlsx
+++ b/Validation/produced_at_day.xlsx
@@ -541,10 +541,10 @@
         <v>0.0001100000000000032</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.0001100000000000026</v>
+        <v>-0.0001099999999965886</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0001100000000000028</v>
+        <v>0.0001099999999969671</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
@@ -560,7 +560,7 @@
         <v>0.004399999999999998</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.0279399999999968</v>
+        <v>-0.02793999999997762</v>
       </c>
       <c r="D7" t="n">
         <v>0.02794000000000001</v>
@@ -579,10 +579,10 @@
         <v>0.004729999999999999</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.01155000000000018</v>
+        <v>-0.01154999999999638</v>
       </c>
       <c r="D8" t="n">
-        <v>0.01155</v>
+        <v>0.01154999999998219</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
@@ -617,10 +617,10 @@
         <v>0.00132</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.001319999999897812</v>
+        <v>-0.001319999999752778</v>
       </c>
       <c r="D10" t="n">
-        <v>0.001319999999893559</v>
+        <v>0.001319999999808475</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -712,10 +712,10 @@
         <v>0.01155</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.2733224999991474</v>
+        <v>-0.2733224999993369</v>
       </c>
       <c r="D15" t="n">
-        <v>0.2733225000002639</v>
+        <v>0.2733224999992497</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
@@ -731,10 +731,10 @@
         <v>0.1141292777775769</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.2856974999996867</v>
+        <v>-0.2856974999988742</v>
       </c>
       <c r="D16" t="n">
-        <v>0.2856974999998592</v>
+        <v>0.2856974999990876</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
@@ -750,10 +750,10 @@
         <v>1.386287414286936</v>
       </c>
       <c r="C17" t="n">
-        <v>1.31084738889111</v>
+        <v>1.31084738888962</v>
       </c>
       <c r="D17" t="n">
-        <v>9.785551111108866</v>
+        <v>9.785551111109099</v>
       </c>
       <c r="E17" t="b">
         <v>1</v>
@@ -769,10 +769,10 @@
         <v>0.01964600000001616</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.03814799999974289</v>
+        <v>-0.0381479999998186</v>
       </c>
       <c r="D18" t="n">
-        <v>0.03814799999924683</v>
+        <v>0.03814800000012006</v>
       </c>
       <c r="E18" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
[UPDATE] reactions validation + [FIX] simulation_sp + PCA + T-SNE + DFA
</commit_message>
<xml_diff>
--- a/Validation/produced_at_day.xlsx
+++ b/Validation/produced_at_day.xlsx
@@ -541,10 +541,10 @@
         <v>0.0001100000000000032</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.0001099999999965886</v>
+        <v>-0.0001100000000000026</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0001099999999969671</v>
+        <v>0.0001100000000000028</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
@@ -560,7 +560,7 @@
         <v>0.004399999999999998</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.02793999999997762</v>
+        <v>-0.0279399999999968</v>
       </c>
       <c r="D7" t="n">
         <v>0.02794000000000001</v>
@@ -579,10 +579,10 @@
         <v>0.004729999999999999</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.01154999999999638</v>
+        <v>-0.01155000000000018</v>
       </c>
       <c r="D8" t="n">
-        <v>0.01154999999998219</v>
+        <v>0.01155</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
@@ -617,10 +617,10 @@
         <v>0.00132</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.001319999999752778</v>
+        <v>-0.001319999999897812</v>
       </c>
       <c r="D10" t="n">
-        <v>0.001319999999808475</v>
+        <v>0.001319999999893559</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -712,10 +712,10 @@
         <v>0.01155</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.2733224999993369</v>
+        <v>-0.2733225000002639</v>
       </c>
       <c r="D15" t="n">
-        <v>0.2733224999992497</v>
+        <v>0.2733225000002639</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
@@ -731,10 +731,10 @@
         <v>0.1141292777775769</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.2856974999988742</v>
+        <v>-0.2856974999997878</v>
       </c>
       <c r="D16" t="n">
-        <v>0.2856974999990876</v>
+        <v>0.2856974999998592</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
@@ -750,10 +750,10 @@
         <v>1.386287414286936</v>
       </c>
       <c r="C17" t="n">
-        <v>1.31084738888962</v>
+        <v>1.310847388890693</v>
       </c>
       <c r="D17" t="n">
-        <v>9.785551111109099</v>
+        <v>9.785551111108866</v>
       </c>
       <c r="E17" t="b">
         <v>1</v>
@@ -769,10 +769,10 @@
         <v>0.01964600000001616</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.0381479999998186</v>
+        <v>-0.03814799999951951</v>
       </c>
       <c r="D18" t="n">
-        <v>0.03814800000012006</v>
+        <v>0.03814799999924683</v>
       </c>
       <c r="E18" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
[FIX] storage pool metabolites (and so, carry out DFA, PCA & T-SNE, validation and simulations again)
</commit_message>
<xml_diff>
--- a/Validation/produced_at_day.xlsx
+++ b/Validation/produced_at_day.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,10 +465,10 @@
         <v>0.02497</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.2960925000002635</v>
+        <v>-0.2960924999994341</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2960925000002595</v>
+        <v>0.2960924999994431</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
@@ -484,10 +484,10 @@
         <v>0.0033</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.003299999999992542</v>
+        <v>-0.0033</v>
       </c>
       <c r="D3" t="n">
-        <v>0.003299999999982353</v>
+        <v>0.0033</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -506,7 +506,7 @@
         <v>-0.0077</v>
       </c>
       <c r="D4" t="n">
-        <v>0.007699999999958584</v>
+        <v>0.0077</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
@@ -519,7 +519,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5.5e-05</v>
+        <v>5.500000000000028e-05</v>
       </c>
       <c r="C5" t="n">
         <v>-5.5e-05</v>
@@ -538,7 +538,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.0001100000000000032</v>
+        <v>0.00011</v>
       </c>
       <c r="C6" t="n">
         <v>-0.0001100000000000026</v>
@@ -557,10 +557,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.004399999999999998</v>
+        <v>0.004400000000000007</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.0279399999999968</v>
+        <v>-0.02794000000000093</v>
       </c>
       <c r="D7" t="n">
         <v>0.02794000000000001</v>
@@ -579,10 +579,10 @@
         <v>0.004729999999999999</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.01155000000000018</v>
+        <v>-0.01154999999999798</v>
       </c>
       <c r="D8" t="n">
-        <v>0.01155</v>
+        <v>0.01155000000000001</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
@@ -610,17 +610,17 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>L-Cysteine_Day_sp_exchange</t>
+          <t>L-Valine_Day_sp_exchange</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.00132</v>
+        <v>0.005500000000000002</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.001319999999897812</v>
+        <v>-0.0209</v>
       </c>
       <c r="D10" t="n">
-        <v>0.001319999999893559</v>
+        <v>0.0209</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -629,17 +629,17 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>L-Glutamine_c_Day_sp_exchange</t>
+          <t>L-Cysteine_Day_sp_exchange</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.1405030523805399</v>
+        <v>0.00132</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.4810767499999504</v>
+        <v>-0.00131999999981512</v>
       </c>
       <c r="D11" t="n">
-        <v>0.4810767500001247</v>
+        <v>0.001319999999866685</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -648,55 +648,55 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>L-Glutamate_c_Day_sp_exchange</t>
+          <t>L-Glutamine_c_Day_sp_exchange</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1.363632861906406</v>
+        <v>0.02048200000000043</v>
       </c>
       <c r="C12" t="n">
-        <v>0.3735187499952807</v>
+        <v>-0.1926048928566449</v>
       </c>
       <c r="D12" t="n">
-        <v>7.024080249999455</v>
+        <v>0.481076749999466</v>
       </c>
       <c r="E12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>L-Tyrosine_Day_sp_exchange</t>
+          <t>L-Glutamate_c_Day_sp_exchange</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.009570000000000002</v>
+        <v>1.416330230160195</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.009569999999987895</v>
+        <v>1.203238055557414</v>
       </c>
       <c r="D13" t="n">
-        <v>0.009570000000015743</v>
+        <v>7.611845999993817</v>
       </c>
       <c r="E13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>L-Asparagine_Day_sp_exchange</t>
+          <t>L-Tyrosine_Day_sp_exchange</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.02145</v>
+        <v>0.009569999999999997</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.1488162499993641</v>
+        <v>-0.009569999999995785</v>
       </c>
       <c r="D14" t="n">
-        <v>0.14881625000023</v>
+        <v>0.009569999999983739</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
@@ -705,17 +705,17 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>L-Serine_c_Day_sp_exchange</t>
+          <t>L-Asparagine_Day_sp_exchange</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.01155</v>
+        <v>0.02145</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.2733225000002639</v>
+        <v>-0.1488162499994153</v>
       </c>
       <c r="D15" t="n">
-        <v>0.2733225000002639</v>
+        <v>0.1488162499996062</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
@@ -724,17 +724,17 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>Starch_p_Day_sp_exchange</t>
+          <t>L-Serine_c_Day_sp_exchange</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.1141292777775769</v>
+        <v>0.01155</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.2856974999997878</v>
+        <v>-0.2733224999990567</v>
       </c>
       <c r="D16" t="n">
-        <v>0.2856974999998592</v>
+        <v>0.2733224999988936</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
@@ -743,38 +743,76 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>(S)-Malate_c_Day_sp_exchange</t>
+          <t>L-Aspartate_c_Day_sp_exchange</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1.386287414286936</v>
+        <v>0.2722904206341817</v>
       </c>
       <c r="C17" t="n">
-        <v>1.310847388890693</v>
+        <v>-4.424533666663168</v>
       </c>
       <c r="D17" t="n">
-        <v>9.785551111108866</v>
+        <v>0.6158618888881841</v>
       </c>
       <c r="E17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
+          <t>Starch_p_Day_sp_exchange</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.1141292777775617</v>
+      </c>
+      <c r="C18" t="n">
+        <v>-0.2856974999999945</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.2609575833331929</v>
+      </c>
+      <c r="E18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>(S)-Malate_c_Day_sp_exchange</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1.073623309526004</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.99116783333576</v>
+      </c>
+      <c r="D19" t="n">
+        <v>9.399136999984796</v>
+      </c>
+      <c r="E19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
           <t>Fumarate_Day_sp_exchange</t>
         </is>
       </c>
-      <c r="B18" t="n">
-        <v>0.01964600000001616</v>
-      </c>
-      <c r="C18" t="n">
-        <v>-0.03814799999951951</v>
-      </c>
-      <c r="D18" t="n">
-        <v>0.03814799999924683</v>
-      </c>
-      <c r="E18" t="b">
+      <c r="B20" t="n">
+        <v>0.0009240000000030056</v>
+      </c>
+      <c r="C20" t="n">
+        <v>-0.03814799999993534</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.03814799999988958</v>
+      </c>
+      <c r="E20" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[ADD] script for validation of reaction fluxes (aragem) + [UPDATE] DFA, reactions validation, PCA&T-SNE and creation for tomato diel model
</commit_message>
<xml_diff>
--- a/Validation/produced_at_day.xlsx
+++ b/Validation/produced_at_day.xlsx
@@ -636,7 +636,7 @@
         <v>0.00132</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.00131999999981512</v>
+        <v>-0.001319999999779366</v>
       </c>
       <c r="D11" t="n">
         <v>0.001319999999866685</v>
@@ -655,7 +655,7 @@
         <v>0.02048200000000043</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.1926048928566449</v>
+        <v>-0.1926048928567539</v>
       </c>
       <c r="D12" t="n">
         <v>0.481076749999466</v>
@@ -674,7 +674,7 @@
         <v>1.416330230160195</v>
       </c>
       <c r="C13" t="n">
-        <v>1.203238055557414</v>
+        <v>1.203238055557247</v>
       </c>
       <c r="D13" t="n">
         <v>7.611845999993817</v>
@@ -693,7 +693,7 @@
         <v>0.009569999999999997</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.009569999999995785</v>
+        <v>-0.009570000000000002</v>
       </c>
       <c r="D14" t="n">
         <v>0.009569999999983739</v>
@@ -715,7 +715,7 @@
         <v>-0.1488162499994153</v>
       </c>
       <c r="D15" t="n">
-        <v>0.1488162499996062</v>
+        <v>0.1488162499994257</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
@@ -734,7 +734,7 @@
         <v>-0.2733224999990567</v>
       </c>
       <c r="D16" t="n">
-        <v>0.2733224999988936</v>
+        <v>0.2733225000000666</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
@@ -753,7 +753,7 @@
         <v>-4.424533666663168</v>
       </c>
       <c r="D17" t="n">
-        <v>0.6158618888881841</v>
+        <v>0.6158618888878094</v>
       </c>
       <c r="E17" t="b">
         <v>0</v>
@@ -772,7 +772,7 @@
         <v>-0.2856974999999945</v>
       </c>
       <c r="D18" t="n">
-        <v>0.2609575833331929</v>
+        <v>0.2609575833332358</v>
       </c>
       <c r="E18" t="b">
         <v>0</v>
@@ -788,7 +788,7 @@
         <v>1.073623309526004</v>
       </c>
       <c r="C19" t="n">
-        <v>0.99116783333576</v>
+        <v>0.9911678333352476</v>
       </c>
       <c r="D19" t="n">
         <v>9.399136999984796</v>
@@ -807,7 +807,7 @@
         <v>0.0009240000000030056</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.03814799999993534</v>
+        <v>-0.03814799999999672</v>
       </c>
       <c r="D20" t="n">
         <v>0.03814799999988958</v>

</xml_diff>